<commit_message>
Moved data to single folder.
Moved data to single overall folder for easier processing. Created .eps figures from matlab .figs. Removed autosave solidworks files. Added test jig to assembly 2.75 (pinned knee). Created folder for figures that will be used in Frontiers knee test paper.
</commit_message>
<xml_diff>
--- a/Testing_Data/2022_02_Festo/Results_table_10mm_pinned_LoadCell.xlsx
+++ b/Testing_Data/2022_02_Festo/Results_table_10mm_pinned_LoadCell.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason Miranda\Documents\GitHub\Bipedal_Robot\Testing_Data\2022_02_Festo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Documents\GitHub\Bipedal_Robot\Testing_Data\2022_02_Festo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4033B40-C8E9-44B1-87E4-1C28A5BE5E38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FC9657AA-55D2-4457-B1D8-BA469ADD9656}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="330" yWindow="375" windowWidth="21600" windowHeight="11385" firstSheet="5" activeTab="8" xr2:uid="{FDAF32CB-2BA8-47E2-927E-3C1E6066A0C3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="4" activeTab="8" xr2:uid="{FDAF32CB-2BA8-47E2-927E-3C1E6066A0C3}"/>
   </bookViews>
   <sheets>
     <sheet name="ExtTest10mm_1" sheetId="9" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <sheet name="FlxTest10mm_3" sheetId="15" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +32,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -3482,6 +3485,101 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.56013262112234863"/>
+                  <c:y val="-0.18098089928539954"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="3"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>ExtTest10mm_6!$C$7:$AE$7</c:f>
@@ -12169,19 +12267,19 @@
         <v>1.2345679012345678E-2</v>
       </c>
       <c r="U22">
-        <f t="shared" ref="U22:X22" si="5">(486-U21)/486</f>
+        <f>(486-U21)/486</f>
         <v>3.292181069958848E-2</v>
       </c>
       <c r="V22">
-        <f t="shared" si="5"/>
+        <f>(486-V21)/486</f>
         <v>7.407407407407407E-2</v>
       </c>
       <c r="W22">
-        <f t="shared" si="5"/>
+        <f>(486-W21)/486</f>
         <v>0.13580246913580246</v>
       </c>
       <c r="X22">
-        <f t="shared" si="5"/>
+        <f>(486-X21)/486</f>
         <v>0.16666666666666666</v>
       </c>
     </row>
@@ -12194,19 +12292,19 @@
         <v>7.407407407407407E-2</v>
       </c>
       <c r="U23">
-        <f t="shared" ref="U23:X23" si="6">U22/$T$26</f>
+        <f>U22/$T$26</f>
         <v>0.19753086419753088</v>
       </c>
       <c r="V23">
-        <f t="shared" si="6"/>
+        <f>V22/$T$26</f>
         <v>0.44444444444444442</v>
       </c>
       <c r="W23">
-        <f t="shared" si="6"/>
+        <f>W22/$T$26</f>
         <v>0.81481481481481477</v>
       </c>
       <c r="X23">
-        <f t="shared" si="6"/>
+        <f>X22/$T$26</f>
         <v>1</v>
       </c>
     </row>
@@ -14675,7 +14773,7 @@
         <v>7.5394492849781658</v>
       </c>
       <c r="E15">
-        <f t="shared" ref="D15:AI15" si="1">E6*SIN(RADIANS(E8))*E12/1000</f>
+        <f t="shared" ref="E15:AI15" si="1">E6*SIN(RADIANS(E8))*E12/1000</f>
         <v>6.6194684828502801</v>
       </c>
       <c r="F15">
@@ -14828,8 +14926,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66E6C766-4925-4D35-B304-44784D2D9843}">
   <dimension ref="A1:Q16"/>
   <sheetViews>
-    <sheetView topLeftCell="D7" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15245,63 +15343,63 @@
         <v>6</v>
       </c>
       <c r="C15">
-        <f>C6*SIN(RADIANS(C8))*C12/1000</f>
+        <f t="shared" ref="C15:Q15" si="0">C6*SIN(RADIANS(C8))*C12/1000</f>
         <v>4.0327772509041173</v>
       </c>
       <c r="D15">
-        <f>D6*SIN(RADIANS(D8))*D12/1000</f>
+        <f t="shared" si="0"/>
         <v>3.7250747045067913</v>
       </c>
       <c r="E15">
-        <f>E6*SIN(RADIANS(E8))*E12/1000</f>
+        <f t="shared" si="0"/>
         <v>3.5012891110164026</v>
       </c>
       <c r="F15">
-        <f>F6*SIN(RADIANS(F8))*F12/1000</f>
+        <f t="shared" si="0"/>
         <v>3.3425458781636546</v>
       </c>
       <c r="G15">
-        <f>G6*SIN(RADIANS(G8))*G12/1000</f>
+        <f t="shared" si="0"/>
         <v>3.0706230541318886</v>
       </c>
       <c r="H15">
-        <f>H6*SIN(RADIANS(H8))*H12/1000</f>
+        <f t="shared" si="0"/>
         <v>2.8447657840215617</v>
       </c>
       <c r="I15">
-        <f>I6*SIN(RADIANS(I8))*I12/1000</f>
+        <f t="shared" si="0"/>
         <v>2.8446217708736867</v>
       </c>
       <c r="J15">
-        <f>J6*SIN(RADIANS(J8))*J12/1000</f>
+        <f t="shared" si="0"/>
         <v>2.7733440251756893</v>
       </c>
       <c r="K15">
-        <f>K6*SIN(RADIANS(K8))*K12/1000</f>
+        <f t="shared" si="0"/>
         <v>2.6744099726497295</v>
       </c>
       <c r="L15">
-        <f>L6*SIN(RADIANS(L8))*L12/1000</f>
+        <f t="shared" si="0"/>
         <v>2.3824102126588129</v>
       </c>
       <c r="M15">
-        <f>M6*SIN(RADIANS(M8))*M12/1000</f>
+        <f t="shared" si="0"/>
         <v>1.6805208635862576</v>
       </c>
       <c r="N15">
-        <f>N6*SIN(RADIANS(N8))*N12/1000</f>
+        <f t="shared" si="0"/>
         <v>0.39482793300422558</v>
       </c>
       <c r="O15">
-        <f>O6*SIN(RADIANS(O8))*O12/1000</f>
+        <f t="shared" si="0"/>
         <v>1.7587132677407729</v>
       </c>
       <c r="P15">
-        <f>P6*SIN(RADIANS(P8))*P12/1000</f>
+        <f t="shared" si="0"/>
         <v>1.550440293736433</v>
       </c>
       <c r="Q15">
-        <f>Q6*SIN(RADIANS(Q8))*Q12/1000</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -15321,7 +15419,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B944D1C8-56B8-47D8-90D4-245D22EBCA01}">
   <dimension ref="A1:AE15"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S14" sqref="S14"/>
     </sheetView>
   </sheetViews>
@@ -15990,7 +16088,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09E5B9E9-F1B4-4DAB-B7CA-9BCB2303132C}">
   <dimension ref="A1:AJ15"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="C13" sqref="C13:AD13"/>
     </sheetView>
   </sheetViews>
@@ -16134,31 +16232,31 @@
         <v>26</v>
       </c>
       <c r="AC5" s="11">
-        <f t="shared" ref="AC5" si="1">AB5+1</f>
+        <f t="shared" ref="AC5:AI5" si="1">AB5+1</f>
         <v>27</v>
       </c>
       <c r="AD5" s="11">
-        <f t="shared" ref="AD5" si="2">AC5+1</f>
+        <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="AE5" s="11">
-        <f t="shared" ref="AE5" si="3">AD5+1</f>
+        <f t="shared" si="1"/>
         <v>29</v>
       </c>
       <c r="AF5" s="11">
-        <f t="shared" ref="AF5" si="4">AE5+1</f>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="AG5" s="11">
-        <f t="shared" ref="AG5" si="5">AF5+1</f>
+        <f t="shared" si="1"/>
         <v>31</v>
       </c>
       <c r="AH5" s="11">
-        <f t="shared" ref="AH5" si="6">AG5+1</f>
+        <f t="shared" si="1"/>
         <v>32</v>
       </c>
       <c r="AI5" s="11">
-        <f t="shared" ref="AI5" si="7">AH5+1</f>
+        <f t="shared" si="1"/>
         <v>33</v>
       </c>
     </row>
@@ -16793,135 +16891,135 @@
         <v>6</v>
       </c>
       <c r="C15">
-        <f t="shared" ref="C15:AI15" si="8">C6*-SIN(RADIANS(C8))*C12/1000</f>
+        <f t="shared" ref="C15:AI15" si="2">C6*-SIN(RADIANS(C8))*C12/1000</f>
         <v>-13.550199438030189</v>
       </c>
       <c r="D15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>-12.715746326203965</v>
       </c>
       <c r="E15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>-12.227450296743585</v>
       </c>
       <c r="F15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>-13.574295183417183</v>
       </c>
       <c r="G15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>-12.617833179689791</v>
       </c>
       <c r="H15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>-11.427173303326315</v>
       </c>
       <c r="I15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>-7.8289359826583684</v>
       </c>
       <c r="J15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>-6.4962395866945686</v>
       </c>
       <c r="K15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>-4.9404873370427511</v>
       </c>
       <c r="L15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>-2.8261340010696823</v>
       </c>
       <c r="M15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>-1.2108000422274927</v>
       </c>
       <c r="N15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>-0.11021594724709009</v>
       </c>
       <c r="O15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>-1.5137448723481624</v>
       </c>
       <c r="P15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>-3.1927408242720881</v>
       </c>
       <c r="Q15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>-4.8615958230354943</v>
       </c>
       <c r="R15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>-6.8694525901110115</v>
       </c>
       <c r="S15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>-8.5997889837959107</v>
       </c>
       <c r="T15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>-10.35823139969961</v>
       </c>
       <c r="U15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>-11.863637901467659</v>
       </c>
       <c r="V15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>-13.477555041999489</v>
       </c>
       <c r="W15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>-13.77813076308844</v>
       </c>
       <c r="X15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>-14.884597105183458</v>
       </c>
       <c r="Y15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>-14.534539473342328</v>
       </c>
       <c r="Z15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>-14.338144060893327</v>
       </c>
       <c r="AA15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>-14.021223986689929</v>
       </c>
       <c r="AB15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>-12.539046654783448</v>
       </c>
       <c r="AC15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>-11.167854768300959</v>
       </c>
       <c r="AD15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>-8.2836070695559112</v>
       </c>
       <c r="AE15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AF15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AG15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AH15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AI15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -16937,7 +17035,7 @@
   <dimension ref="A1:AJ29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17805,8 +17903,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB28D160-17A5-469E-8CF6-067E3CB95279}">
   <dimension ref="A1:AJ29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C15" activeCellId="1" sqref="C7:L7 C15:L15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Removed extra trend lines
</commit_message>
<xml_diff>
--- a/Testing_Data/2022_02_Festo/Results_table_10mm_pinned_LoadCell.xlsx
+++ b/Testing_Data/2022_02_Festo/Results_table_10mm_pinned_LoadCell.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Documents\GitHub\Bipedal_Robot\Testing_Data\2022_02_Festo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FC9657AA-55D2-4457-B1D8-BA469ADD9656}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08F0557B-4C61-477A-8262-2AB215425F0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="4" activeTab="8" xr2:uid="{FDAF32CB-2BA8-47E2-927E-3C1E6066A0C3}"/>
+    <workbookView minimized="1" xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="10980" firstSheet="4" activeTab="4" xr2:uid="{FDAF32CB-2BA8-47E2-927E-3C1E6066A0C3}"/>
   </bookViews>
   <sheets>
     <sheet name="ExtTest10mm_1" sheetId="9" r:id="rId1"/>
@@ -3550,6 +3550,12 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.30954483814523187"/>
+                  <c:y val="-2.5762248468941384E-2"/>
+                </c:manualLayout>
+              </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -4133,6 +4139,20 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:trendlineType val="log"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:trendlineType val="poly"/>
             <c:order val="3"/>
             <c:dispRSqr val="1"/>
@@ -4140,8 +4160,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.40464027934008251"/>
-                  <c:y val="-1.2615056781268678E-2"/>
+                  <c:x val="-0.27899278215223094"/>
+                  <c:y val="0.3201971535736251"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -4173,35 +4193,6 @@
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
-          </c:trendline>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="log"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="poly"/>
-            <c:order val="5"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -4801,6 +4792,20 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:trendlineType val="log"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:trendlineType val="poly"/>
             <c:order val="3"/>
             <c:dispRSqr val="1"/>
@@ -4808,8 +4813,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.40464027934008251"/>
-                  <c:y val="-1.2615056781268678E-2"/>
+                  <c:x val="-0.40762374401637524"/>
+                  <c:y val="4.5584595515824444E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -4841,35 +4846,6 @@
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
-          </c:trendline>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="log"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="poly"/>
-            <c:order val="5"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -10995,16 +10971,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>740833</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>7937</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>74612</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>131233</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>331258</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>36512</xdr:rowOff>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -14926,8 +14902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66E6C766-4925-4D35-B304-44784D2D9843}">
   <dimension ref="A1:Q16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16088,7 +16064,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09E5B9E9-F1B4-4DAB-B7CA-9BCB2303132C}">
   <dimension ref="A1:AJ15"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13:AD13"/>
     </sheetView>
   </sheetViews>
@@ -17035,7 +17011,7 @@
   <dimension ref="A1:AJ29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17903,7 +17879,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB28D160-17A5-469E-8CF6-067E3CB95279}">
   <dimension ref="A1:AJ29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Working on wrapping point locations for pinned extensor tests
</commit_message>
<xml_diff>
--- a/Testing_Data/2022_02_Festo/Results_table_10mm_pinned_LoadCell.xlsx
+++ b/Testing_Data/2022_02_Festo/Results_table_10mm_pinned_LoadCell.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Documents\GitHub\Bipedal_Robot\Testing_Data\2022_02_Festo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Bipedal_Robot\Testing_Data\2022_02_Festo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E5560F8-6F0F-41EC-9B10-4B2993FA0E07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC201AFB-FDB5-4A0E-92A4-37E860E17DC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35970" yWindow="30" windowWidth="21630" windowHeight="11250" firstSheet="2" activeTab="3" xr2:uid="{FDAF32CB-2BA8-47E2-927E-3C1E6066A0C3}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{FDAF32CB-2BA8-47E2-927E-3C1E6066A0C3}"/>
   </bookViews>
   <sheets>
     <sheet name="ExtTest10mm_1" sheetId="9" r:id="rId1"/>
@@ -23,28 +23,17 @@
     <sheet name="FlxTest10mm_2" sheetId="8" r:id="rId8"/>
     <sheet name="FlxTest10mm_3" sheetId="15" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="47">
   <si>
     <t>Test #</t>
   </si>
@@ -182,6 +171,9 @@
   </si>
   <si>
     <t>original</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -1857,123 +1849,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-0.60346456692913386"/>
-                  <c:y val="-0.28313193524076818"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="poly"/>
-            <c:order val="3"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-0.40464027934008251"/>
-                  <c:y val="-1.2615056781268678E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
             <c:trendlineType val="log"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="poly"/>
-            <c:order val="5"/>
             <c:dispRSqr val="0"/>
             <c:dispEq val="0"/>
           </c:trendline>
@@ -3444,56 +3320,6 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-0.56013262112234863"/>
-                  <c:y val="-0.18098089928539954"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
           <c:trendline>
             <c:spPr>
               <a:ln w="19050" cap="rnd">
@@ -11299,7 +11125,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -11313,24 +11139,24 @@
       <selection activeCell="C6" sqref="C6:K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="3"/>
-    <col min="2" max="2" width="19.6640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" customWidth="1"/>
-    <col min="5" max="5" width="8.6640625" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" customWidth="1"/>
-    <col min="8" max="9" width="13.44140625" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="2" max="2" width="19.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" customWidth="1"/>
+    <col min="8" max="9" width="13.42578125" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -11341,7 +11167,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>14</v>
       </c>
@@ -11350,7 +11176,7 @@
         <v>403.38</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>17</v>
       </c>
@@ -11358,7 +11184,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="5" spans="1:36" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:36" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>0</v>
       </c>
@@ -11481,7 +11307,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>1</v>
       </c>
@@ -11546,7 +11372,7 @@
         <v>23.167999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
         <v>2</v>
       </c>
@@ -11611,7 +11437,7 @@
         <v>-123</v>
       </c>
     </row>
-    <row r="8" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>7</v>
       </c>
@@ -11679,13 +11505,13 @@
         <v>84.4</v>
       </c>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
       <c r="B9" s="8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
       <c r="B10" s="8" t="s">
         <v>3</v>
@@ -11765,7 +11591,7 @@
       <c r="AI10" s="2"/>
       <c r="AJ10" s="2"/>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>8</v>
       </c>
@@ -11791,7 +11617,7 @@
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
       <c r="B12" s="8" t="s">
         <v>10</v>
@@ -11866,7 +11692,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="8" t="s">
         <v>11</v>
@@ -11932,13 +11758,13 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13"/>
       <c r="B14" s="9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>6</v>
       </c>
@@ -12075,12 +11901,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="3:24" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="3:24" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C18">
         <f>C6+4.6262</f>
         <v>22.176200000000001</v>
@@ -12118,7 +11944,7 @@
         <v>6.3061999999999996</v>
       </c>
     </row>
-    <row r="19" spans="3:24" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C19">
         <v>22.176200000000001</v>
       </c>
@@ -12147,12 +11973,12 @@
         <v>6.3061999999999996</v>
       </c>
     </row>
-    <row r="20" spans="3:24" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="3:24" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C21">
         <v>17.55</v>
       </c>
@@ -12181,7 +12007,7 @@
         <v>1.68</v>
       </c>
     </row>
-    <row r="22" spans="3:24" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:24" x14ac:dyDescent="0.25">
       <c r="T22">
         <v>480</v>
       </c>
@@ -12198,7 +12024,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="23" spans="3:24" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:24" x14ac:dyDescent="0.25">
       <c r="S23" t="s">
         <v>30</v>
       </c>
@@ -12223,7 +12049,7 @@
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="24" spans="3:24" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:24" x14ac:dyDescent="0.25">
       <c r="S24" t="s">
         <v>31</v>
       </c>
@@ -12248,7 +12074,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="3:24" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:24" x14ac:dyDescent="0.25">
       <c r="S27" t="s">
         <v>32</v>
       </c>
@@ -12272,24 +12098,24 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="3"/>
-    <col min="2" max="2" width="19.6640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" customWidth="1"/>
-    <col min="5" max="5" width="8.6640625" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" customWidth="1"/>
-    <col min="8" max="9" width="13.44140625" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="2" max="2" width="19.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" customWidth="1"/>
+    <col min="8" max="9" width="13.42578125" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -12300,7 +12126,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>14</v>
       </c>
@@ -12309,7 +12135,7 @@
         <v>379.31</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>17</v>
       </c>
@@ -12321,7 +12147,7 @@
         <v>0.16849015317286653</v>
       </c>
     </row>
-    <row r="5" spans="1:36" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:36" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>0</v>
       </c>
@@ -12444,7 +12270,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>1</v>
       </c>
@@ -12536,7 +12362,7 @@
         <v>24.667000000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
         <v>2</v>
       </c>
@@ -12628,7 +12454,7 @@
         <v>-123</v>
       </c>
     </row>
-    <row r="8" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>7</v>
       </c>
@@ -12723,13 +12549,13 @@
         <v>81.400000000000006</v>
       </c>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
       <c r="B9" s="8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
       <c r="B10" s="8" t="s">
         <v>3</v>
@@ -12827,7 +12653,7 @@
       <c r="AI10" s="2"/>
       <c r="AJ10" s="2"/>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>8</v>
       </c>
@@ -12853,7 +12679,7 @@
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
       <c r="B12" s="8" t="s">
         <v>10</v>
@@ -12958,7 +12784,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="8" t="s">
         <v>11</v>
@@ -13051,13 +12877,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13"/>
       <c r="B14" s="9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>6</v>
       </c>
@@ -13209,24 +13035,24 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="3"/>
-    <col min="2" max="2" width="19.6640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" customWidth="1"/>
-    <col min="5" max="5" width="8.6640625" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" customWidth="1"/>
-    <col min="8" max="9" width="13.44140625" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="2" max="2" width="19.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" customWidth="1"/>
+    <col min="8" max="9" width="13.42578125" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -13237,7 +13063,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>14</v>
       </c>
@@ -13246,7 +13072,7 @@
         <v>403.38</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>17</v>
       </c>
@@ -13258,7 +13084,7 @@
         <v>0.18106995884773658</v>
       </c>
     </row>
-    <row r="5" spans="1:36" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:36" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>0</v>
       </c>
@@ -13381,7 +13207,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>1</v>
       </c>
@@ -13398,7 +13224,7 @@
         <v>13.111000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
         <v>2</v>
       </c>
@@ -13415,7 +13241,7 @@
         <v>-92</v>
       </c>
     </row>
-    <row r="8" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>7</v>
       </c>
@@ -13435,13 +13261,13 @@
         <v>80.7</v>
       </c>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
       <c r="B9" s="8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
       <c r="B10" s="8" t="s">
         <v>3</v>
@@ -13489,7 +13315,7 @@
       <c r="AI10" s="2"/>
       <c r="AJ10" s="2"/>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>8</v>
       </c>
@@ -13515,7 +13341,7 @@
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
       <c r="B12" s="8" t="s">
         <v>10</v>
@@ -13620,7 +13446,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="8" t="s">
         <v>11</v>
@@ -13638,13 +13464,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13"/>
       <c r="B14" s="9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>6</v>
       </c>
@@ -13792,28 +13618,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D539E524-5F19-4B4B-B21A-C95F2596B6A0}">
   <dimension ref="A1:AJ27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AC18" sqref="AC18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="3"/>
-    <col min="2" max="2" width="19.6640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" customWidth="1"/>
-    <col min="5" max="5" width="8.6640625" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" customWidth="1"/>
-    <col min="8" max="9" width="13.44140625" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="2" max="2" width="19.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" customWidth="1"/>
+    <col min="8" max="9" width="13.42578125" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -13824,7 +13650,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>14</v>
       </c>
@@ -13836,7 +13662,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>17</v>
       </c>
@@ -13857,7 +13683,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:36" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:36" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>0</v>
       </c>
@@ -13980,7 +13806,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>1</v>
       </c>
@@ -14066,7 +13892,7 @@
         <v>33.061999999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
         <v>2</v>
       </c>
@@ -14149,7 +13975,7 @@
         <v>-66</v>
       </c>
     </row>
-    <row r="8" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>7</v>
       </c>
@@ -14235,13 +14061,13 @@
         <v>83.5</v>
       </c>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
       <c r="B9" s="8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
       <c r="B10" s="8" t="s">
         <v>3</v>
@@ -14333,7 +14159,7 @@
       <c r="AI10" s="2"/>
       <c r="AJ10" s="2"/>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>8</v>
       </c>
@@ -14359,7 +14185,7 @@
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
       <c r="B12" s="8" t="s">
         <v>10</v>
@@ -14464,7 +14290,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="8" t="s">
         <v>11</v>
@@ -14548,13 +14374,13 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13"/>
       <c r="B14" s="9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>6</v>
       </c>
@@ -14691,7 +14517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
       <c r="U16" t="s">
         <v>23</v>
       </c>
@@ -14699,22 +14525,22 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="17:29" x14ac:dyDescent="0.3">
+    <row r="17" spans="17:29" x14ac:dyDescent="0.25">
       <c r="AB17">
         <v>2.2241</v>
       </c>
     </row>
-    <row r="18" spans="17:29" x14ac:dyDescent="0.3">
+    <row r="18" spans="17:29" x14ac:dyDescent="0.25">
       <c r="AC18" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="17:29" x14ac:dyDescent="0.3">
+    <row r="24" spans="17:29" x14ac:dyDescent="0.25">
       <c r="Q24" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="17:29" x14ac:dyDescent="0.3">
+    <row r="25" spans="17:29" x14ac:dyDescent="0.25">
       <c r="Q25" t="s">
         <v>42</v>
       </c>
@@ -14725,7 +14551,7 @@
         <v>-1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="26" spans="17:29" x14ac:dyDescent="0.3">
+    <row r="26" spans="17:29" x14ac:dyDescent="0.25">
       <c r="Q26" t="s">
         <v>43</v>
       </c>
@@ -14736,7 +14562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="17:29" x14ac:dyDescent="0.3">
+    <row r="27" spans="17:29" x14ac:dyDescent="0.25">
       <c r="R27">
         <v>505</v>
       </c>
@@ -14752,28 +14578,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66E6C766-4925-4D35-B304-44784D2D9843}">
   <dimension ref="A1:Q16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="3"/>
-    <col min="2" max="2" width="19.6640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" customWidth="1"/>
-    <col min="5" max="5" width="8.6640625" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" customWidth="1"/>
-    <col min="8" max="9" width="13.44140625" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="2" max="2" width="19.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" customWidth="1"/>
+    <col min="8" max="9" width="13.42578125" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -14784,7 +14610,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>36</v>
       </c>
@@ -14792,7 +14618,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>35</v>
       </c>
@@ -14803,7 +14629,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>0</v>
       </c>
@@ -14853,7 +14679,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>1</v>
       </c>
@@ -14900,7 +14726,7 @@
         <v>6.2092000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
         <v>2</v>
       </c>
@@ -14947,7 +14773,7 @@
         <v>-18.5</v>
       </c>
     </row>
-    <row r="8" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>7</v>
       </c>
@@ -14997,7 +14823,7 @@
         <v>90.5</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
       <c r="B9" s="8" t="s">
         <v>3</v>
@@ -15035,8 +14861,8 @@
       <c r="M9">
         <v>363</v>
       </c>
-      <c r="N9">
-        <v>340</v>
+      <c r="N9" t="s">
+        <v>46</v>
       </c>
       <c r="O9">
         <v>355</v>
@@ -15045,7 +14871,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="10" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>8</v>
       </c>
@@ -15053,13 +14879,13 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="12"/>
       <c r="B11" s="8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
       <c r="B12" s="8" t="s">
         <v>10</v>
@@ -15110,7 +14936,7 @@
         <v>249.71</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="8" t="s">
         <v>11</v>
@@ -15158,13 +14984,13 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13"/>
       <c r="B14" s="9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>6</v>
       </c>
@@ -15229,7 +15055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="L16" t="s">
         <v>39</v>
       </c>
@@ -15246,27 +15072,27 @@
   <dimension ref="A1:AE15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="3"/>
-    <col min="2" max="2" width="19.6640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" customWidth="1"/>
-    <col min="5" max="5" width="8.6640625" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" customWidth="1"/>
-    <col min="8" max="9" width="13.44140625" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="2" max="2" width="19.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" customWidth="1"/>
+    <col min="8" max="9" width="13.42578125" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -15277,7 +15103,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>36</v>
       </c>
@@ -15285,7 +15111,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>35</v>
       </c>
@@ -15293,7 +15119,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:31" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:31" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>0</v>
       </c>
@@ -15385,7 +15211,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>1</v>
       </c>
@@ -15441,7 +15267,7 @@
         <v>17.72</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
         <v>2</v>
       </c>
@@ -15497,7 +15323,7 @@
         <v>-119.5</v>
       </c>
     </row>
-    <row r="8" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>7</v>
       </c>
@@ -15556,7 +15382,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
       <c r="B9" s="8" t="s">
         <v>3</v>
@@ -15613,7 +15439,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="10" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>8</v>
       </c>
@@ -15621,13 +15447,13 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" s="12"/>
       <c r="B11" s="8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
       <c r="B12" s="8" t="s">
         <v>10</v>
@@ -15720,7 +15546,7 @@
         <v>249.71</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="8" t="s">
         <v>11</v>
@@ -15777,13 +15603,13 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13"/>
       <c r="B14" s="9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>6</v>
       </c>
@@ -15919,24 +15745,24 @@
       <selection activeCell="C13" sqref="C13:AD13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="3"/>
-    <col min="2" max="2" width="19.6640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" customWidth="1"/>
-    <col min="5" max="5" width="8.6640625" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" customWidth="1"/>
-    <col min="8" max="9" width="13.44140625" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="2" max="2" width="19.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" customWidth="1"/>
+    <col min="8" max="9" width="13.42578125" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -15947,7 +15773,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>14</v>
       </c>
@@ -15956,7 +15782,7 @@
         <v>402.55</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>17</v>
       </c>
@@ -15964,7 +15790,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="5" spans="1:36" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:36" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>0</v>
       </c>
@@ -16087,7 +15913,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>1</v>
       </c>
@@ -16176,7 +16002,7 @@
         <v>30.405999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
         <v>2</v>
       </c>
@@ -16265,7 +16091,7 @@
         <v>19.5</v>
       </c>
     </row>
-    <row r="8" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>7</v>
       </c>
@@ -16357,13 +16183,13 @@
         <v>118.5</v>
       </c>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
       <c r="B9" s="8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
       <c r="B10" s="8" t="s">
         <v>3</v>
@@ -16459,7 +16285,7 @@
       <c r="AI10" s="2"/>
       <c r="AJ10" s="2"/>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>8</v>
       </c>
@@ -16485,7 +16311,7 @@
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
       <c r="B12" s="8" t="s">
         <v>10</v>
@@ -16575,7 +16401,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="8" t="s">
         <v>11</v>
@@ -16665,13 +16491,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13"/>
       <c r="B14" s="9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>6</v>
       </c>
@@ -16823,24 +16649,24 @@
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="3"/>
-    <col min="2" max="2" width="19.6640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" customWidth="1"/>
-    <col min="5" max="5" width="8.6640625" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" customWidth="1"/>
-    <col min="8" max="9" width="13.44140625" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="2" max="2" width="19.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" customWidth="1"/>
+    <col min="8" max="9" width="13.42578125" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -16851,7 +16677,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>14</v>
       </c>
@@ -16863,7 +16689,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>17</v>
       </c>
@@ -16874,7 +16700,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:36" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:36" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>0</v>
       </c>
@@ -16997,7 +16823,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>1</v>
       </c>
@@ -17062,7 +16888,7 @@
         <v>48.012999999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
         <v>2</v>
       </c>
@@ -17127,7 +16953,7 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="8" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>7</v>
       </c>
@@ -17195,13 +17021,13 @@
         <v>95.1</v>
       </c>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
       <c r="B9" s="8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
       <c r="B10" s="8" t="s">
         <v>3</v>
@@ -17281,7 +17107,7 @@
       <c r="AI10" s="2"/>
       <c r="AJ10" s="2"/>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>8</v>
       </c>
@@ -17307,7 +17133,7 @@
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
       <c r="B12" s="8" t="s">
         <v>10</v>
@@ -17412,7 +17238,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="8" t="s">
         <v>11</v>
@@ -17478,13 +17304,13 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13"/>
       <c r="B14" s="9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>6</v>
       </c>
@@ -17621,12 +17447,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
       <c r="L16" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="18:18" x14ac:dyDescent="0.3">
+    <row r="29" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R29">
         <f>485*1.03</f>
         <v>499.55</v>
@@ -17647,24 +17473,24 @@
       <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="3"/>
-    <col min="2" max="2" width="19.6640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" customWidth="1"/>
-    <col min="5" max="5" width="8.6640625" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" customWidth="1"/>
-    <col min="8" max="9" width="13.44140625" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="2" max="2" width="19.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" customWidth="1"/>
+    <col min="8" max="9" width="13.42578125" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -17675,7 +17501,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>14</v>
       </c>
@@ -17684,7 +17510,7 @@
         <v>379.31</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>17</v>
       </c>
@@ -17692,7 +17518,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="5" spans="1:36" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:36" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>0</v>
       </c>
@@ -17815,7 +17641,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>1</v>
       </c>
@@ -17850,7 +17676,7 @@
         <v>2.0994000000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
         <v>2</v>
       </c>
@@ -17885,7 +17711,7 @@
         <v>-105</v>
       </c>
     </row>
-    <row r="8" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>7</v>
       </c>
@@ -17923,13 +17749,13 @@
         <v>76.599999999999994</v>
       </c>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
       <c r="B9" s="8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
       <c r="B10" s="8" t="s">
         <v>3</v>
@@ -17989,7 +17815,7 @@
       <c r="AI10" s="2"/>
       <c r="AJ10" s="2"/>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>8</v>
       </c>
@@ -18015,7 +17841,7 @@
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
       <c r="B12" s="8" t="s">
         <v>10</v>
@@ -18120,7 +17946,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="8" t="s">
         <v>11</v>
@@ -18156,13 +17982,13 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13"/>
       <c r="B14" s="9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>6</v>
       </c>
@@ -18299,13 +18125,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="10:18" x14ac:dyDescent="0.3">
+    <row r="18" spans="10:18" x14ac:dyDescent="0.25">
       <c r="J18">
         <f>1-348/457</f>
         <v>0.23851203501094087</v>
       </c>
     </row>
-    <row r="29" spans="10:18" x14ac:dyDescent="0.3">
+    <row r="29" spans="10:18" x14ac:dyDescent="0.25">
       <c r="R29">
         <f>485*1.03</f>
         <v>499.55</v>

</xml_diff>